<commit_message>
column names made unique
</commit_message>
<xml_diff>
--- a/master_sheet_reference.xlsx
+++ b/master_sheet_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade.sharepoint.com/sites/SUIT/Shared Documents/00_SUIT INFRA PROJECTS/24_8163.001 PIF COE PL and TT/01-Project Lighthouse/30-WIP/50-Dashboard/Working Dashboard Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68208164-FD91-4403-A269-DB8B92E1C047}"/>
+  <xr:revisionPtr revIDLastSave="395" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F3EA5C-A96B-4980-A106-A87F7CA57D13}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="6" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="93">
   <si>
     <t>Visual</t>
   </si>
@@ -285,12 +285,6 @@
     <t>Audits/Inspections</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Remaining Planned</t>
   </si>
   <si>
@@ -316,6 +310,21 @@
   </si>
   <si>
     <t>Budget Value (Forecast) in M SAR</t>
+  </si>
+  <si>
+    <t>Value_training</t>
+  </si>
+  <si>
+    <t>In Progress_audits</t>
+  </si>
+  <si>
+    <t>Completed_audits</t>
+  </si>
+  <si>
+    <t>In Progress_actions</t>
+  </si>
+  <si>
+    <t>Completed_actions</t>
   </si>
 </sst>
 </file>
@@ -323,7 +332,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$$-C09]#,##0;[Red]\-[$$-C09]#,##0"/>
+    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0;[Red]\-[$$-C09]#,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -349,30 +358,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -386,20 +377,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:B8"/>
     </sheetView>
   </sheetViews>
@@ -1186,7 +1176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1194,7 +1184,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1202,7 +1192,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1210,7 +1200,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1218,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1226,7 +1216,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1256,7 +1246,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,7 +1335,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1353,7 +1343,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1361,24 +1351,16 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1402,7 +1384,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,58 +1426,58 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1521,7 +1503,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,79 +1534,80 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
+      <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
-        <v>86</v>
+      <c r="B10" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1663,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64CC8F8-7393-471E-9562-88A0C3211012}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,10 +1661,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="1"/>
@@ -1690,140 +1673,160 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1847,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1871,39 +1874,39 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
@@ -1911,7 +1914,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -1919,10 +1922,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data pull across all tabs. Updated AG and master ref 19/5
</commit_message>
<xml_diff>
--- a/master_sheet_reference.xlsx
+++ b/master_sheet_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="395" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F3EA5C-A96B-4980-A106-A87F7CA57D13}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F86C815-4A55-4AF1-A14F-4072064CD740}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>DevCoAssessmentAnalysis(I&amp;T)</t>
   </si>
   <si>
-    <t>PerformanceSignal</t>
-  </si>
-  <si>
     <t>Budget Value (Baseline) in M SAR</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>Completed_actions</t>
+  </si>
+  <si>
+    <t>Performance Signal</t>
   </si>
 </sst>
 </file>
@@ -379,17 +379,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,99 +724,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="C9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1098,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:B8"/>
     </sheetView>
   </sheetViews>
@@ -1246,7 +1249,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="A13:B14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1338,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,7 +1346,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1351,16 +1354,14 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1426,58 +1427,58 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1503,7 +1504,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,80 +1535,79 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>84</v>
+      <c r="B10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64CC8F8-7393-471E-9562-88A0C3211012}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -1661,10 +1661,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="1"/>
@@ -1673,160 +1673,140 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1850,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1881,26 +1861,26 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1925,7 +1905,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with new dashboards
</commit_message>
<xml_diff>
--- a/master_sheet_reference.xlsx
+++ b/master_sheet_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="422" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9701CC22-1D09-4FC0-9937-E0D493A404A7}"/>
+  <xr:revisionPtr revIDLastSave="478" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE5F9F7F-C820-4E6E-88E4-B2DB11A58D40}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="7" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="28695" yWindow="75" windowWidth="14370" windowHeight="15585" firstSheet="9" activeTab="9" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="102">
   <si>
     <t>Visual</t>
   </si>
@@ -334,6 +334,24 @@
   </si>
   <si>
     <t>DevCoAssessmentInput(D&amp;T)</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Pending (Ha)</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentAnalysis(S&amp;O)</t>
+  </si>
+  <si>
+    <t>AddDataPoint(S&amp;O)</t>
+  </si>
+  <si>
+    <t>Weightage</t>
+  </si>
+  <si>
+    <t>Name of the KPI</t>
   </si>
 </sst>
 </file>
@@ -853,14 +871,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -871,18 +890,54 @@
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10561AED-7A60-4961-BD19-7A4144646A11}">
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
@@ -1938,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34921496-A0A7-47F9-8DE9-DF05A8622000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,14 +2089,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535A6DC-85F0-42C2-9B34-850413E49A7C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2052,11 +2109,79 @@
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated reference file with updated columns
</commit_message>
<xml_diff>
--- a/master_sheet_reference.xlsx
+++ b/master_sheet_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="481" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{240AAC9A-E9AC-419E-B61A-5120A7E34399}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1212AA9D-963B-4DF1-AB51-868F9B4F1C14}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="75" windowWidth="14370" windowHeight="15585" firstSheet="9" activeTab="7" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="108">
   <si>
     <t>Table</t>
   </si>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t>Word Cloud</t>
+  </si>
+  <si>
+    <t>Position Vacant</t>
+  </si>
+  <si>
+    <t>Position Missing</t>
+  </si>
+  <si>
+    <t>Name of the Policy</t>
+  </si>
+  <si>
+    <t>Criticality (Y/N)</t>
+  </si>
+  <si>
+    <t>Availability (Y/N)</t>
+  </si>
+  <si>
+    <t>Name of the Technical Platform</t>
   </si>
 </sst>
 </file>
@@ -361,7 +379,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0;[Red]\-[$$-C09]#,##0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,16 +773,16 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -775,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -786,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -797,7 +815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -806,7 +824,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -815,7 +833,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -824,7 +842,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -833,7 +851,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -842,7 +860,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -871,19 +889,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,7 +912,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -901,7 +920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -909,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -917,7 +936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -925,12 +944,92 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -958,197 +1057,197 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -1169,14 +1268,14 @@
       <selection activeCell="A7" sqref="A7:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.9">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.9">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1203,7 +1302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1211,7 +1310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1219,7 +1318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1227,7 +1326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.9">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.9">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1243,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1267,7 +1366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1283,7 +1382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1316,13 +1415,13 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.9">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1341,7 +1440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.9">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1349,7 +1448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.9">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.9">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1365,7 +1464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.9">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1397,7 +1496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1405,7 +1504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1413,7 +1512,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1421,10 +1520,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
   </sheetData>
@@ -1452,15 +1551,15 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1482,7 +1581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1490,7 +1589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1498,7 +1597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1506,7 +1605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1514,7 +1613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1530,7 +1629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1538,7 +1637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1571,14 +1670,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1598,7 +1697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1606,12 +1705,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1619,7 +1718,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1627,7 +1726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1635,7 +1734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1643,7 +1742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1651,7 +1750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1659,7 +1758,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1667,7 +1766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +1774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1683,7 +1782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1716,15 +1815,15 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1744,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1752,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1760,7 +1859,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1768,7 +1867,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1776,7 +1875,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1784,7 +1883,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1792,7 +1891,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1800,7 +1899,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1808,7 +1907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1824,7 +1923,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1832,7 +1931,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1840,7 +1939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1848,7 +1947,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1856,7 +1955,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1864,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1898,14 +1997,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1916,7 +2015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1924,7 +2023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1932,7 +2031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1940,7 +2039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1948,7 +2047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1956,7 +2055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1964,7 +2063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1993,18 +2092,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34921496-A0A7-47F9-8DE9-DF05A8622000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +2113,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2022,7 +2121,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2030,7 +2129,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -2038,7 +2137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2046,7 +2145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -2054,7 +2153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2062,7 +2161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2070,7 +2169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2103,14 +2202,14 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2219,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2128,7 +2227,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2136,7 +2235,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2144,7 +2243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -2152,7 +2251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2160,7 +2259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2168,7 +2267,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2176,7 +2275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2184,7 +2283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>

</xml_diff>